<commit_message>
added functionality to burger
</commit_message>
<xml_diff>
--- a/Munros.xlsx
+++ b/Munros.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fergu\Documents\Work\munro-site\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D22F880-5E33-4D98-9A65-62D8693AE824}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908FB086-FF79-48C6-92C0-9DC70E533647}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DF2BA6AB-DE0A-4591-B698-D10C46D2B2A0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="299">
   <si>
     <t>Munros</t>
   </si>
@@ -96,9 +96,6 @@
     <t>Ben More</t>
   </si>
   <si>
-    <t>Ben Avon (Leabaidh an Daimh Bhuidhe</t>
-  </si>
-  <si>
     <t>Stob Binnein</t>
   </si>
   <si>
@@ -928,6 +925,12 @@
   </si>
   <si>
     <t>Crieff</t>
+  </si>
+  <si>
+    <t>Ben Avon (Leabaidh an Daimh Bhuidhe)</t>
+  </si>
+  <si>
+    <t>Sgurr Mor (Loch Quoich)</t>
   </si>
 </sst>
 </file>
@@ -1299,8 +1302,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A7F9488-69B7-40AB-95B8-87CFE5BB7707}">
   <dimension ref="A1:I284"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A193" workbookViewId="0">
-      <selection activeCell="A71" sqref="A71"/>
+    <sheetView tabSelected="1" topLeftCell="A257" workbookViewId="0">
+      <selection activeCell="A284" sqref="A284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1319,10 +1322,10 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C1" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -1331,21 +1334,21 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>284</v>
+      </c>
+      <c r="G1" t="s">
         <v>285</v>
       </c>
-      <c r="G1" t="s">
-        <v>286</v>
-      </c>
       <c r="H1" t="s">
+        <v>290</v>
+      </c>
+      <c r="I1" t="s">
         <v>291</v>
-      </c>
-      <c r="I1" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D2">
         <v>936</v>
@@ -1356,7 +1359,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D3">
         <v>997</v>
@@ -1367,7 +1370,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D4">
         <v>930</v>
@@ -1378,7 +1381,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D5">
         <v>1120</v>
@@ -1389,7 +1392,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D6">
         <v>918</v>
@@ -1400,7 +1403,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D7">
         <v>967</v>
@@ -1411,7 +1414,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D8">
         <v>975</v>
@@ -1422,7 +1425,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D9">
         <v>934</v>
@@ -1433,7 +1436,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D10">
         <v>1032</v>
@@ -1444,7 +1447,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D11">
         <v>954</v>
@@ -1455,10 +1458,10 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B12" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C12">
         <v>4</v>
@@ -1484,7 +1487,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="D13">
         <v>923</v>
@@ -1495,7 +1498,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D14">
         <v>982</v>
@@ -1506,7 +1509,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15">
         <v>1129</v>
@@ -1517,7 +1520,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D16">
         <v>1006</v>
@@ -1528,7 +1531,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D17">
         <v>1069</v>
@@ -1539,7 +1542,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="D18">
         <v>944</v>
@@ -1550,7 +1553,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D19">
         <v>921</v>
@@ -1561,7 +1564,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D20">
         <v>1118</v>
@@ -1572,7 +1575,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D21">
         <v>1021</v>
@@ -1594,7 +1597,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D23">
         <v>1116</v>
@@ -1605,7 +1608,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D24">
         <v>1001</v>
@@ -1638,7 +1641,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27">
         <v>1083</v>
@@ -1649,7 +1652,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D28">
         <v>1049</v>
@@ -1660,7 +1663,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D29">
         <v>1087</v>
@@ -1671,10 +1674,10 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B30" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C30">
         <v>7</v>
@@ -1700,7 +1703,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D31">
         <v>980</v>
@@ -1711,7 +1714,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D32">
         <v>1081</v>
@@ -1722,10 +1725,10 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B33" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C33">
         <v>4</v>
@@ -1751,7 +1754,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D34">
         <v>1038</v>
@@ -1762,7 +1765,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D35">
         <v>1004</v>
@@ -1773,7 +1776,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D36">
         <v>1019</v>
@@ -1784,7 +1787,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D37">
         <v>931</v>
@@ -1795,7 +1798,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D38">
         <v>1157</v>
@@ -1806,10 +1809,10 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B39" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C39">
         <v>3</v>
@@ -1832,10 +1835,10 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B40" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C40">
         <v>4</v>
@@ -1861,7 +1864,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D41">
         <v>1008</v>
@@ -1872,7 +1875,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D42">
         <v>1084</v>
@@ -1883,7 +1886,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D43">
         <v>1076</v>
@@ -1894,10 +1897,10 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B44" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C44">
         <v>8</v>
@@ -1923,7 +1926,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D45">
         <v>1102</v>
@@ -1934,7 +1937,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D46">
         <v>989</v>
@@ -1945,7 +1948,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D47">
         <v>1032</v>
@@ -1956,7 +1959,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D48">
         <v>1005</v>
@@ -1967,7 +1970,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D49">
         <v>959</v>
@@ -1978,7 +1981,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D50">
         <v>1103</v>
@@ -1989,7 +1992,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D51">
         <v>1078</v>
@@ -2000,10 +2003,10 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B52" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -2026,7 +2029,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D53">
         <v>1045</v>
@@ -2037,10 +2040,10 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B54" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C54">
         <v>7</v>
@@ -2066,7 +2069,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D55">
         <v>926</v>
@@ -2077,7 +2080,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="D56">
         <v>954</v>
@@ -2088,7 +2091,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="D57">
         <v>954</v>
@@ -2110,7 +2113,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D59">
         <v>935</v>
@@ -2121,7 +2124,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D60">
         <v>960</v>
@@ -2132,10 +2135,10 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B61" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C61">
         <v>2</v>
@@ -2158,7 +2161,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D62">
         <v>974</v>
@@ -2169,7 +2172,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D63">
         <v>937</v>
@@ -2180,7 +2183,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D64">
         <v>937</v>
@@ -2191,7 +2194,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D65">
         <v>915</v>
@@ -2202,10 +2205,10 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B66" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C66">
         <v>5</v>
@@ -2231,7 +2234,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D67">
         <v>1011</v>
@@ -2242,7 +2245,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D68">
         <v>1148</v>
@@ -2253,7 +2256,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>20</v>
+        <v>297</v>
       </c>
       <c r="D69">
         <v>1171</v>
@@ -2264,7 +2267,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="D70">
         <v>1025</v>
@@ -2275,10 +2278,10 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B71" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C71">
         <v>10</v>
@@ -2304,7 +2307,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D72">
         <v>1126</v>
@@ -2315,7 +2318,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D73">
         <v>927</v>
@@ -2326,7 +2329,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D74">
         <v>962</v>
@@ -2348,10 +2351,10 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B76" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C76">
         <v>1</v>
@@ -2388,7 +2391,7 @@
         <v>19</v>
       </c>
       <c r="B78" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C78">
         <v>6</v>
@@ -2414,7 +2417,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D79">
         <v>966</v>
@@ -2425,7 +2428,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D80">
         <v>998</v>
@@ -2447,10 +2450,10 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B82" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="C82">
         <v>8</v>
@@ -2476,7 +2479,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D83">
         <v>1078</v>
@@ -2487,10 +2490,10 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B84" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C84">
         <v>2</v>
@@ -2513,10 +2516,10 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B85" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C85">
         <v>9</v>
@@ -2542,10 +2545,10 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B86" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="C86">
         <v>3</v>
@@ -2568,7 +2571,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D87">
         <v>1046</v>
@@ -2579,7 +2582,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D88">
         <v>1150</v>
@@ -2590,7 +2593,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="D89">
         <v>945</v>
@@ -2601,7 +2604,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D90">
         <v>1062</v>
@@ -2612,7 +2615,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D91">
         <v>943</v>
@@ -2623,7 +2626,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D92">
         <v>1130</v>
@@ -2634,7 +2637,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D93">
         <v>928</v>
@@ -2656,7 +2659,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D95">
         <v>1070</v>
@@ -2667,7 +2670,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D96">
         <v>998</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D97">
         <v>958</v>
@@ -2694,7 +2697,7 @@
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D99">
         <v>1090</v>
@@ -2705,7 +2708,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D100">
         <v>1012</v>
@@ -2727,7 +2730,7 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D102">
         <v>1064</v>
@@ -2749,7 +2752,7 @@
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D104">
         <v>963</v>
@@ -2760,7 +2763,7 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D105">
         <v>1110</v>
@@ -2771,7 +2774,7 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D106">
         <v>975</v>
@@ -2782,7 +2785,7 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D107">
         <v>1037</v>
@@ -2793,7 +2796,7 @@
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D108">
         <v>994</v>
@@ -2804,7 +2807,7 @@
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D109">
         <v>1029</v>
@@ -2815,7 +2818,7 @@
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D110">
         <v>1047</v>
@@ -2826,7 +2829,7 @@
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D111">
         <v>1019</v>
@@ -2837,7 +2840,7 @@
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D112">
         <v>917</v>
@@ -2848,7 +2851,7 @@
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D113">
         <v>946</v>
@@ -2859,7 +2862,7 @@
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D114">
         <v>941</v>
@@ -2870,7 +2873,7 @@
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D115">
         <v>1034</v>
@@ -2881,7 +2884,7 @@
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D116">
         <v>945</v>
@@ -2903,7 +2906,7 @@
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D118">
         <v>957</v>
@@ -2914,7 +2917,7 @@
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D119">
         <v>1029</v>
@@ -2925,7 +2928,7 @@
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D120">
         <v>975</v>
@@ -2936,7 +2939,7 @@
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="D121">
         <v>1006</v>
@@ -2947,7 +2950,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D122">
         <v>1041</v>
@@ -2969,7 +2972,7 @@
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="D124">
         <v>941</v>
@@ -2980,7 +2983,7 @@
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D125">
         <v>1121</v>
@@ -2991,7 +2994,7 @@
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D126">
         <v>992</v>
@@ -3002,7 +3005,7 @@
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D127">
         <v>992</v>
@@ -3013,7 +3016,7 @@
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="D128">
         <v>920</v>
@@ -3024,7 +3027,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D129">
         <v>1046</v>
@@ -3035,7 +3038,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D130">
         <v>979</v>
@@ -3046,7 +3049,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D131">
         <v>978</v>
@@ -3057,7 +3060,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D132">
         <v>987</v>
@@ -3068,7 +3071,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D133">
         <v>947</v>
@@ -3079,7 +3082,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D134">
         <v>987</v>
@@ -3090,7 +3093,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D135">
         <v>1128</v>
@@ -3101,7 +3104,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D136">
         <v>1047</v>
@@ -3112,7 +3115,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D137">
         <v>918</v>
@@ -3123,7 +3126,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="D138">
         <v>924</v>
@@ -3134,7 +3137,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D139">
         <v>1100</v>
@@ -3145,10 +3148,10 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B140" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C140">
         <v>5</v>
@@ -3174,7 +3177,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D141">
         <v>1155</v>
@@ -3185,7 +3188,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D142">
         <v>947</v>
@@ -3196,7 +3199,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D143">
         <v>987</v>
@@ -3207,7 +3210,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D144">
         <v>927</v>
@@ -3218,7 +3221,7 @@
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D145">
         <v>933</v>
@@ -3229,7 +3232,7 @@
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D146">
         <v>919</v>
@@ -3240,7 +3243,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D147">
         <v>1013</v>
@@ -3251,7 +3254,7 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D148">
         <v>917</v>
@@ -3262,7 +3265,7 @@
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D149">
         <v>1049</v>
@@ -3273,7 +3276,7 @@
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D150">
         <v>926</v>
@@ -3284,7 +3287,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D151">
         <v>1132</v>
@@ -3295,7 +3298,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D152">
         <v>997</v>
@@ -3306,7 +3309,7 @@
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D153">
         <v>1068</v>
@@ -3317,7 +3320,7 @@
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="D154">
         <v>1051</v>
@@ -3328,7 +3331,7 @@
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D155">
         <v>1035</v>
@@ -3339,7 +3342,7 @@
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D156">
         <v>987</v>
@@ -3350,7 +3353,7 @@
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D157">
         <v>986</v>
@@ -3361,7 +3364,7 @@
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D158">
         <v>1020</v>
@@ -3372,7 +3375,7 @@
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D159">
         <v>1155</v>
@@ -3383,7 +3386,7 @@
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D160">
         <v>939</v>
@@ -3394,7 +3397,7 @@
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D161">
         <v>986</v>
@@ -3416,7 +3419,7 @@
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D163">
         <v>1007</v>
@@ -3427,7 +3430,7 @@
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D164">
         <v>933</v>
@@ -3438,7 +3441,7 @@
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D165">
         <v>981</v>
@@ -3449,7 +3452,7 @@
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="D166">
         <v>928</v>
@@ -3460,7 +3463,7 @@
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D167">
         <v>1108</v>
@@ -3471,7 +3474,7 @@
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="D168">
         <v>926</v>
@@ -3482,7 +3485,7 @@
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D169">
         <v>934</v>
@@ -3493,7 +3496,7 @@
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D170">
         <v>932</v>
@@ -3504,7 +3507,7 @@
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D171">
         <v>946</v>
@@ -3515,7 +3518,7 @@
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D172">
         <v>951</v>
@@ -3526,7 +3529,7 @@
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D173">
         <v>1069</v>
@@ -3537,7 +3540,7 @@
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D174">
         <v>953</v>
@@ -3548,7 +3551,7 @@
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D175">
         <v>1118</v>
@@ -3559,7 +3562,7 @@
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D176">
         <v>968</v>
@@ -3570,7 +3573,7 @@
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D177">
         <v>1039</v>
@@ -3581,7 +3584,7 @@
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A178" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D178">
         <v>959</v>
@@ -3592,7 +3595,7 @@
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A179" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D179">
         <v>949</v>
@@ -3603,7 +3606,7 @@
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A180" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D180">
         <v>1001</v>
@@ -3614,7 +3617,7 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D181">
         <v>918</v>
@@ -3625,7 +3628,7 @@
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A182" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D182">
         <v>981</v>
@@ -3636,7 +3639,7 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A183" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D183">
         <v>977</v>
@@ -3647,7 +3650,7 @@
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A184" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="D184">
         <v>928</v>
@@ -3658,7 +3661,7 @@
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A185" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D185">
         <v>1044</v>
@@ -3669,7 +3672,7 @@
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A186" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D186">
         <v>1113</v>
@@ -3680,7 +3683,7 @@
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A187" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D187">
         <v>928</v>
@@ -3691,7 +3694,7 @@
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A188" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D188">
         <v>939</v>
@@ -3702,7 +3705,7 @@
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A189" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D189">
         <v>1023</v>
@@ -3713,7 +3716,7 @@
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A190" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D190">
         <v>1019</v>
@@ -3724,7 +3727,7 @@
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A191" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D191">
         <v>1018</v>
@@ -3735,7 +3738,7 @@
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D192">
         <v>1102</v>
@@ -3746,7 +3749,7 @@
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A193" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D193">
         <v>982</v>
@@ -3757,7 +3760,7 @@
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A194" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D194">
         <v>939</v>
@@ -3768,7 +3771,7 @@
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D195">
         <v>1056</v>
@@ -3779,7 +3782,7 @@
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A196" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D196">
         <v>918</v>
@@ -3790,7 +3793,7 @@
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A197" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D197">
         <v>1010</v>
@@ -3801,7 +3804,7 @@
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D198">
         <v>1002</v>
@@ -3812,7 +3815,7 @@
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A199" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D199">
         <v>956</v>
@@ -3823,7 +3826,7 @@
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A200" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D200">
         <v>1083</v>
@@ -3834,7 +3837,7 @@
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="D201">
         <v>927</v>
@@ -3845,7 +3848,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A202" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D202">
         <v>991</v>
@@ -3856,7 +3859,7 @@
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D203">
         <v>921</v>
@@ -3878,7 +3881,7 @@
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="D205">
         <v>955</v>
@@ -3889,7 +3892,7 @@
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A206" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D206">
         <v>1118</v>
@@ -3900,7 +3903,7 @@
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A207" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D207">
         <v>994</v>
@@ -3911,7 +3914,7 @@
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A208" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D208">
         <v>1024</v>
@@ -3922,7 +3925,7 @@
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A209" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D209">
         <v>1001</v>
@@ -3933,7 +3936,7 @@
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A210" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D210">
         <v>962</v>
@@ -3944,7 +3947,7 @@
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A211" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D211">
         <v>967</v>
@@ -3955,7 +3958,7 @@
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A212" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D212">
         <v>1036</v>
@@ -3966,7 +3969,7 @@
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A213" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D213">
         <v>1053</v>
@@ -3977,7 +3980,7 @@
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A214" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D214">
         <v>1083</v>
@@ -3988,7 +3991,7 @@
     </row>
     <row r="215" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A215" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D215">
         <v>973</v>
@@ -3999,7 +4002,7 @@
     </row>
     <row r="216" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A216" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D216">
         <v>918</v>
@@ -4010,7 +4013,7 @@
     </row>
     <row r="217" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A217" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D217">
         <v>1099</v>
@@ -4021,7 +4024,7 @@
     </row>
     <row r="218" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D218">
         <v>1027</v>
@@ -4032,7 +4035,7 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A219" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D219">
         <v>992</v>
@@ -4043,7 +4046,7 @@
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A220" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D220">
         <v>1010</v>
@@ -4054,7 +4057,7 @@
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A221" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D221">
         <v>1004</v>
@@ -4065,7 +4068,7 @@
     </row>
     <row r="222" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D222">
         <v>989</v>
@@ -4076,7 +4079,7 @@
     </row>
     <row r="223" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A223" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D223">
         <v>999</v>
@@ -4087,7 +4090,7 @@
     </row>
     <row r="224" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A224" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D224">
         <v>999</v>
@@ -4098,7 +4101,7 @@
     </row>
     <row r="225" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A225" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D225">
         <v>1094</v>
@@ -4109,7 +4112,7 @@
     </row>
     <row r="226" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A226" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="D226">
         <v>944</v>
@@ -4120,7 +4123,7 @@
     </row>
     <row r="227" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A227" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D227">
         <v>1010</v>
@@ -4131,7 +4134,7 @@
     </row>
     <row r="228" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A228" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D228">
         <v>1067</v>
@@ -4142,7 +4145,7 @@
     </row>
     <row r="229" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A229" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D229">
         <v>1049</v>
@@ -4153,7 +4156,7 @@
     </row>
     <row r="230" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A230" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D230">
         <v>1060</v>
@@ -4164,7 +4167,7 @@
     </row>
     <row r="231" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A231" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D231">
         <v>948</v>
@@ -4175,7 +4178,7 @@
     </row>
     <row r="232" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A232" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D232">
         <v>986</v>
@@ -4186,7 +4189,7 @@
     </row>
     <row r="233" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A233" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D233">
         <v>1110</v>
@@ -4197,7 +4200,7 @@
     </row>
     <row r="234" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A234" t="s">
-        <v>46</v>
+        <v>298</v>
       </c>
       <c r="D234">
         <v>1003</v>
@@ -4208,7 +4211,7 @@
     </row>
     <row r="235" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A235" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D235">
         <v>965</v>
@@ -4219,7 +4222,7 @@
     </row>
     <row r="236" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A236" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D236">
         <v>1002</v>
@@ -4230,7 +4233,7 @@
     </row>
     <row r="237" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A237" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D237">
         <v>1027</v>
@@ -4241,7 +4244,7 @@
     </row>
     <row r="238" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A238" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D238">
         <v>1040</v>
@@ -4252,7 +4255,7 @@
     </row>
     <row r="239" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A239" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D239">
         <v>1150</v>
@@ -4263,7 +4266,7 @@
     </row>
     <row r="240" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A240" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D240">
         <v>993</v>
@@ -4274,7 +4277,7 @@
     </row>
     <row r="241" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A241" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="D241">
         <v>946</v>
@@ -4285,7 +4288,7 @@
     </row>
     <row r="242" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A242" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D242">
         <v>1151</v>
@@ -4296,7 +4299,7 @@
     </row>
     <row r="243" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A243" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D243">
         <v>1093</v>
@@ -4307,7 +4310,7 @@
     </row>
     <row r="244" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A244" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D244">
         <v>953</v>
@@ -4318,7 +4321,7 @@
     </row>
     <row r="245" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A245" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D245">
         <v>956</v>
@@ -4329,7 +4332,7 @@
     </row>
     <row r="246" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A246" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D246">
         <v>1109</v>
@@ -4340,7 +4343,7 @@
     </row>
     <row r="247" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A247" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D247">
         <v>923</v>
@@ -4351,7 +4354,7 @@
     </row>
     <row r="248" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A248" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="D248">
         <v>924</v>
@@ -4362,7 +4365,7 @@
     </row>
     <row r="249" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A249" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D249">
         <v>964</v>
@@ -4373,7 +4376,7 @@
     </row>
     <row r="250" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A250" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D250">
         <v>963</v>
@@ -4384,7 +4387,7 @@
     </row>
     <row r="251" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A251" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D251">
         <v>993</v>
@@ -4395,7 +4398,7 @@
     </row>
     <row r="252" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A252" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D252">
         <v>981</v>
@@ -4406,7 +4409,7 @@
     </row>
     <row r="253" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A253" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D253">
         <v>1055</v>
@@ -4417,7 +4420,7 @@
     </row>
     <row r="254" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A254" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D254">
         <v>996</v>
@@ -4428,7 +4431,7 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A255" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D255">
         <v>937</v>
@@ -4439,7 +4442,7 @@
     </row>
     <row r="256" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A256" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D256">
         <v>1105</v>
@@ -4450,7 +4453,7 @@
     </row>
     <row r="257" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A257" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D257">
         <v>945</v>
@@ -4461,7 +4464,7 @@
     </row>
     <row r="258" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A258" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D258">
         <v>999</v>
@@ -4472,7 +4475,7 @@
     </row>
     <row r="259" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A259" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D259">
         <v>977</v>
@@ -4483,10 +4486,10 @@
     </row>
     <row r="260" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A260" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B260" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="C260">
         <v>6</v>
@@ -4523,7 +4526,7 @@
     </row>
     <row r="262" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A262" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D262">
         <v>1044</v>
@@ -4534,7 +4537,7 @@
     </row>
     <row r="263" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A263" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D263">
         <v>981</v>
@@ -4545,7 +4548,7 @@
     </row>
     <row r="264" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A264" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D264">
         <v>1116</v>
@@ -4556,7 +4559,7 @@
     </row>
     <row r="265" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A265" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D265">
         <v>1115</v>
@@ -4567,7 +4570,7 @@
     </row>
     <row r="266" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A266" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D266">
         <v>925</v>
@@ -4578,7 +4581,7 @@
     </row>
     <row r="267" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A267" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D267">
         <v>1072</v>
@@ -4589,7 +4592,7 @@
     </row>
     <row r="268" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A268" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D268">
         <v>979</v>
@@ -4600,7 +4603,7 @@
     </row>
     <row r="269" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A269" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D269">
         <v>1021</v>
@@ -4611,7 +4614,7 @@
     </row>
     <row r="270" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A270" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D270">
         <v>998</v>
@@ -4622,7 +4625,7 @@
     </row>
     <row r="271" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A271" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D271">
         <v>958</v>
@@ -4633,7 +4636,7 @@
     </row>
     <row r="272" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A272" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D272">
         <v>1090</v>
@@ -4644,7 +4647,7 @@
     </row>
     <row r="273" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A273" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D273">
         <v>956</v>
@@ -4655,7 +4658,7 @@
     </row>
     <row r="274" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A274" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="D274">
         <v>1054</v>
@@ -4666,10 +4669,10 @@
     </row>
     <row r="275" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A275" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B275" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C275">
         <v>9</v>
@@ -4695,7 +4698,7 @@
     </row>
     <row r="276" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A276" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D276">
         <v>960</v>
@@ -4706,7 +4709,7 @@
     </row>
     <row r="277" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A277" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D277">
         <v>933</v>
@@ -4717,7 +4720,7 @@
     </row>
     <row r="278" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A278" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D278">
         <v>1004</v>
@@ -4728,7 +4731,7 @@
     </row>
     <row r="279" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A279" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D279">
         <v>1010</v>
@@ -4739,7 +4742,7 @@
     </row>
     <row r="280" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A280" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D280">
         <v>1054</v>
@@ -4750,7 +4753,7 @@
     </row>
     <row r="281" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A281" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D281">
         <v>958</v>
@@ -4761,7 +4764,7 @@
     </row>
     <row r="282" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A282" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D282">
         <v>1112</v>
@@ -4772,7 +4775,7 @@
     </row>
     <row r="283" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A283" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D283">
         <v>957</v>
@@ -4783,7 +4786,7 @@
     </row>
     <row r="284" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D284">
         <v>922</v>

</xml_diff>